<commit_message>
writing more Tese Cases for Register page
</commit_message>
<xml_diff>
--- a/OpenCart_TestCases.xlsx
+++ b/OpenCart_TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="436"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289"/>
   </bookViews>
   <sheets>
     <sheet name="Registration_Page" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>Product Name</t>
   </si>
@@ -169,6 +169,195 @@
 2. Validate the email subject, email body and from email address of the received email
 3. Validate there is a link to the Login page provided in the Email body
 4. User should be taken to the Login page  </t>
+  </si>
+  <si>
+    <t>TC_RF_003</t>
+  </si>
+  <si>
+    <t>TC_RF_004</t>
+  </si>
+  <si>
+    <t>Validate all the requirement fields are present in the registration form</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option
+3. Check all the require fields (ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should see all the mandatory fields First Name, Last Name, E-Mail,Telephone, Password, Password Confirm and  Privacy Policy Fields</t>
+  </si>
+  <si>
+    <t>Validate registering an account by providing all the fields</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' drop menu
+2. Click on 'Register' option
+3. Enter First Name, Last Name, E-Mail,Telephone, Password, Password Confirm and  Privacy Policy Fields
+4. Click 'Continue' button (ER-1)
+5. Click 'Continue' button that is displayed 'Registration Successful' page (ER-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be logged in, taken to 'Account Success' page and proper details should be displayed on the page
+2. User should be taken to 'Account' page </t>
+  </si>
+  <si>
+    <t>TC_RF_005</t>
+  </si>
+  <si>
+    <t>Check 'Privacy Policy' checkbox is not selected by default and without checkin this checkbox account should not create.</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' drop menu
+2. Click on 'Register' option
+3. Check the 'Privacy Policy' Checkbox (ER-1)
+4. Click on 'Continue' button (ER-2)</t>
+  </si>
+  <si>
+    <t>1. 'Privacy Policy' Checkbox should not checked by default
+2. User should can't create an account</t>
+  </si>
+  <si>
+    <t>TC_RF_006</t>
+  </si>
+  <si>
+    <t>Validate registering an account when 'Yes' option is selected for 'Newsletter' field</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm and  Privacy Policy Fields)
+4.Click on 'Yes' radio option for Newsletter 
+5. Click on 'Continue' button (ER-1)
+6. Click on 'Continue' button that is displayed in the 'Account Success' page (ER-2)
+7. Click on 'Subscribe/unsubscribe to newsletter' option (ER-3)</t>
+  </si>
+  <si>
+    <t>1. User should be logged in,  taken to 'Account Succcess' page and proper details should be displayed on the page
+2. User should be taken to 'Account' page 
+3. 'Yes' option should be displayed as selected by default in the Newsletter page</t>
+  </si>
+  <si>
+    <t>TC_RF_007</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account when 'No' option is selected for Newsletter field</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm and  Privacy Policy Fields)
+4.Click on 'No'  radio option for Newsletter 
+5. Click on 'Continue' button (ER-1)
+6. Click on 'Continue' button that is displayed in the 'Account Success' page (ER-2)
+7. Click on 'Subscribe/unsubscribe to newsletter' option (ER-3)</t>
+  </si>
+  <si>
+    <t>1. User should be logged in,  taken to 'Account Succcess' page and proper details should be displayed on the page
+2. User should be taken to 'Account' page 
+3. 'No' option should be displayed as selected by default in the Newsletter page</t>
+  </si>
+  <si>
+    <t>TC_RF_008</t>
+  </si>
+  <si>
+    <t>Validate different ways of navigating to 'Register Account' page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'My Account' Drop menu
+2. Click on 'Register' option (ER-1) 
+3. Click on 'My Account' Drop menu
+4. Click on 'Login' option 
+5. Click  on 'Continue' button inside 'New Customer' box (ER-1) 
+6. Repeat Steps 3 and 4
+7. Click on 'Register' option from the Right Column options (ER-1) </t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Register Account' page</t>
+  </si>
+  <si>
+    <t>TC_RF_009</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account by entering different passwords into 'Password' and 'Password Confirm' fields</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Newsletter and  Privacy Policy Fields)
+4. Enter any password say '12345' into the 'Password' field
+5. Enter any different password say 'abcde' into the 'Passsword Confirm' field
+6. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1.Account should not be created, instead a warning message - 'Password confirmation does not match password!' should be displayed under 'Password Confirm' field</t>
+  </si>
+  <si>
+    <t>TC_RF_010</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account by providing the existing account details</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter existing Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm, Newsletter and  Privacy Policy Fields) - &lt;Refer Test Data&gt;
+4. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>First Name - Mehedi
+Last Name - Rony
+E-Mail - rony@gmail.com
+Telephone - 90909****
+Password - 12345
+Password Confirm - 12345</t>
+  </si>
+  <si>
+    <t>1. Account should not be created again, instead the warning messsage -  'Warning: E-Mail Address is already registered!' should be displayed</t>
+  </si>
+  <si>
+    <t>TC_RF_011</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account by providing an invalid email address into the E-Mail field</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name,Telephone, Password, Password Confirm, Newsletter and  Privacy Policy Fields) 
+4. Enter invalid email address into the E-Mail Field - &lt;Refer Test Data&gt;
+5. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>Try all below invalid email address formats:
+1) mehedi
+2) rony@
+3) r@gmail
+4) r@gail.com</t>
+  </si>
+  <si>
+    <t>1. Account should not be created, instead a proper field level warning message or page level warning message to provide valid email address should be displayed</t>
+  </si>
+  <si>
+    <t>TC_RF_012</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account by providing an invalid phone number</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new  Account Details into all the Fields (First Name, Last Name,E-Mail, Password, Password Confirm, Newsletter and  Privacy Policy Fields)
+4. Enter invalid phone number into the Telephone Field - &lt;Refer Test Data&gt;
+5. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>Try all below invalid phone formats:
+1) 111
+2) abcde</t>
+  </si>
+  <si>
+    <t>1. Account should not be created, instead a proper warning message should be displayed</t>
   </si>
 </sst>
 </file>
@@ -458,9 +647,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -469,9 +656,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -479,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -563,32 +748,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,7 +1088,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +1108,7 @@
     <col min="2" max="2" width="38.26953125" customWidth="1"/>
     <col min="3" max="3" width="46.08984375" customWidth="1"/>
     <col min="4" max="4" width="37.81640625" customWidth="1"/>
-    <col min="5" max="5" width="34.81640625" customWidth="1"/>
+    <col min="5" max="5" width="43.453125" customWidth="1"/>
     <col min="6" max="6" width="31.1796875" customWidth="1"/>
     <col min="7" max="7" width="34.81640625" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
@@ -925,10 +1116,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
@@ -942,16 +1133,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="36"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="21" t="s">
         <v>30</v>
       </c>
@@ -969,8 +1160,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -990,10 +1181,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1015,17 +1206,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
@@ -1060,15 +1251,31 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="35" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:9" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:9" s="32" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" s="29" customFormat="1" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>34</v>
@@ -1083,21 +1290,174 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="40" customFormat="1" ht="158" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="32" customFormat="1" ht="158" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="33" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="31" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="32" customFormat="1" ht="150.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="32" customFormat="1" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="32" customFormat="1" ht="206" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="32" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="32" customFormat="1" ht="218.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="32" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="32" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="32" customFormat="1" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="32" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more Test Cases added to Register Account Page
</commit_message>
<xml_diff>
--- a/OpenCart_TestCases.xlsx
+++ b/OpenCart_TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>Product Name</t>
   </si>
@@ -358,6 +358,152 @@
   </si>
   <si>
     <t>1. Account should not be created, instead a proper warning message should be displayed</t>
+  </si>
+  <si>
+    <t>TC_RF_013</t>
+  </si>
+  <si>
+    <t>Validate Registering an Account by using the Keyboard keys</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm, Newsletter and  Privacy Policy Fields) by using Keyboard keys (Tab, Spacebar and Enter)
+4. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be logged in,  taken to 'Account Succcess' page and proper details should be displayed on the page</t>
+  </si>
+  <si>
+    <t>TC_RF_014</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Check the Fields - First Name, Last Name, E-Mail, Telephone, Password, Password Confirm and Privacy Policy</t>
+  </si>
+  <si>
+    <t>Validate all the mandatory fields in the Register Account page are marked with red color ' * ' symbol</t>
+  </si>
+  <si>
+    <t>All the specified fields in the Test steps should be marked with red color * symbol.</t>
+  </si>
+  <si>
+    <t>TC_RF_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate wheather the mandatory fields in the Register Account page are accepting only spaces. </t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter spaces into the Mandatory Fields (First Name, Last Name, E-Mail,Telephone, Password and Password Confirm)
+4. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. Warning message should be displayed for the mandatory fields.</t>
+  </si>
+  <si>
+    <t>TC_RF_016</t>
+  </si>
+  <si>
+    <t>Validate wheather the password field of the Register Account page is following the password complexity standard.</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Newsletter and  Privacy Policy Fields)
+4. Check entering simple passwords (Not following Password Complexity Standars' i.e. Size of password as 8, password should contain atleat one number, symbol, lower case letter and upper case letters) - &lt;Refer Test Data&gt;
+5. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. Warning message should be displayed for following Password Complexity Standards</t>
+  </si>
+  <si>
+    <t>TC_RF_017</t>
+  </si>
+  <si>
+    <t>Validate whether the fields in the Register Account page are according the Client requirements (Examples- Height, Width, Number of characters etc.)</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Check all the fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm, Newsletter and  Privacy Policy Fields) including the 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. Text fields should abide to the Client requirements</t>
+  </si>
+  <si>
+    <t>TC_RF_018</t>
+  </si>
+  <si>
+    <t>Validate the 'Password' and 'Confirm Password' fields in the 'Register Account' page are abide to the functionality of toggle to hide and toggole to visibility</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter some Password text into the 'Password' and 'Password Confirm' fields (ER-1)</t>
+  </si>
+  <si>
+    <t>1.Password text entered into 'Password' and 'Confirm Password' fields need to be toggled to hide its visibilty (It should be hidden by displaying * or . Symbols)</t>
+  </si>
+  <si>
+    <t>TC_RF_019</t>
+  </si>
+  <si>
+    <t>Validate registering an account by filling the 'Password' field but not filling the 'Confirm Password' field.</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Newsletter and  Privacy Policy Fields)
+4. Don't enter into 'Password Confirm' field
+5. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. Warning message - 'Password confirmation does not match password!' should be displayed under 'Password Confirm' field</t>
+  </si>
+  <si>
+    <t>TC_RF_020</t>
+  </si>
+  <si>
+    <t>Validate navigeting to other pages by using the options or links provided on the 'Register Account' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Try clicking on 'login page' link, 'privacy policy' link, 'Right Column' options, Menu options, Header and Footer options and any other options</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to the respective pages without any problems</t>
+  </si>
+  <si>
+    <t>TC_RF_021</t>
+  </si>
+  <si>
+    <t>Validate the responsiveness of 'Register Account' page in different browsers</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option</t>
+  </si>
+  <si>
+    <t>Proper and require UI should be displayed on different browsers like Google chrome, Mozilla firefox, Opera mini etc</t>
+  </si>
+  <si>
+    <t>TC_RF_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the details that are provided while Registering an Account are stored in the Database </t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Drop menu
+2. Click on 'Register' option 
+3. Enter new Account Details into all the Fields (First Name, Last Name, E-Mail,Telephone, Password, Password Confirm, Newsletter and  Privacy Policy Fields)
+4. Click on 'Continue' button (ER-1)</t>
+  </si>
+  <si>
+    <t>1. All the details entered while registering the account are successfully stored in the Database</t>
   </si>
 </sst>
 </file>
@@ -664,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -755,11 +901,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -769,17 +927,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1088,7 +1237,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1096,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1116,10 +1265,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
@@ -1133,16 +1282,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="37"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="21" t="s">
         <v>30</v>
       </c>
@@ -1160,8 +1309,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -1181,10 +1330,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1206,17 +1355,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
@@ -1251,8 +1400,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
+    <row r="7" spans="1:9" s="40" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1325,7 +1474,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="32" customFormat="1" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="34" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="31" t="s">
@@ -1359,7 +1508,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" s="32" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B14" s="31" t="s">
@@ -1376,19 +1525,19 @@
       </c>
     </row>
     <row r="15" spans="1:9" s="32" customFormat="1" ht="218.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="35" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="35" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1410,10 +1559,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="32" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -1422,15 +1571,15 @@
       <c r="D17" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="32" customFormat="1" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="35" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="31" t="s">
@@ -1439,15 +1588,15 @@
       <c r="D18" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="35" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="32" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="35" t="s">
         <v>82</v>
       </c>
       <c r="C19" s="31" t="s">
@@ -1456,8 +1605,178 @@
       <c r="D19" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="35" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="32" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="32" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="32" customFormat="1" ht="125.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="32" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="27">
+        <v>12345</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="32" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="32" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="32" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="32" customFormat="1" ht="127" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="32" customFormat="1" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="32" customFormat="1" ht="120.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test cases for Logout functionality
</commit_message>
<xml_diff>
--- a/OpenCart_TestCases.xlsx
+++ b/OpenCart_TestCases.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Login_Page" sheetId="2" r:id="rId2"/>
+    <sheet name="Logout_Page" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="317">
   <si>
     <t>Product Name</t>
   </si>
@@ -1054,12 +1055,192 @@
 4) Ronyol@gmail.com
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">Test Scenario </t>
+  </si>
+  <si>
+    <t>Pre-requisites</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>TC_LG_001</t>
+  </si>
+  <si>
+    <t>(TS_003)
+Logout Functionality</t>
+  </si>
+  <si>
+    <t>Validate Logging out by selecting Logout option from 'My Account' dropmenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL
+2. User is logged in
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Logout' option (Verify ER-1)
+3. Click on 'Continue' button (Verify ER-2)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to the 'Account Logout' page and User should see Login option inplace of Logout under the 'My Account' dropmenu
+2. User should be taken to the Home page</t>
+  </si>
+  <si>
+    <t>TC_LG_002</t>
+  </si>
+  <si>
+    <t>Validate Logging out by selecting Logout option from 'Right Column' options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL
+2. User is logged in and is on 'Account' page
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'Logout' option from the Right Column  (Verify ER-1)
+2. Click on 'Continue' button (Verify ER-2)</t>
+  </si>
+  <si>
+    <t>TC_LG_003</t>
+  </si>
+  <si>
+    <t>Validate the Application session status, after logging and closing the Browser without logging out</t>
+  </si>
+  <si>
+    <t>1. Close the Browser without Logging out
+2. Open the Browser and navigate the application (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Application should not get logged out, instead the user loggedin session need to be mainitained</t>
+  </si>
+  <si>
+    <t>TC_LG_004</t>
+  </si>
+  <si>
+    <t>Validate logging out and browsing back</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Logout' option
+3. Click on Browser back button (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should not get logged in</t>
+  </si>
+  <si>
+    <t>TC_LG_005</t>
+  </si>
+  <si>
+    <t>Validate Logout option is not displayed under 'My Account' menu before logging in</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu  (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Logout option should not be displayed under 'My Account' dropmenu</t>
+  </si>
+  <si>
+    <t>TC_LG_006</t>
+  </si>
+  <si>
+    <t>Validate Logout option is not displayed under 'Right Column' options before logging in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application </t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Regiser' option (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Logout option should not be displayed in the 'Right Column'</t>
+  </si>
+  <si>
+    <t>TC_LG_007</t>
+  </si>
+  <si>
+    <t>Validate logout from an Account from a single place after logging into it from different places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL
+2. User is logged in Firefox Browser of your laptop
+3. User is logged in with the same acccount of step2 in Chrome browser of your Mobile device
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu in Firefox Browser
+2. Select 'Logout' option
+3. Perform any operation which requires the user to log, say navigating to Address Book page in the Chrome Browser of Mobile device (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. User be logged out in Mobile device too, instead of getting navigated to the Address book page</t>
+  </si>
+  <si>
+    <t>TC_LG_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate logging out and loggin in immediately after logout </t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Logout' option
+3. Login immediately again with same or different account (Verify ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Same Account or Differnet Account should get loggedin </t>
+  </si>
+  <si>
+    <t>TC_LG_009</t>
+  </si>
+  <si>
+    <t>Validate 'Account Logout' page</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL
+2. User is logged in</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Logout' option
+3. Check the Page Heading, Page Title, Page URL and Breadcrumb of the displayed 'Account Logout' page (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper Page Heading, Page Title, Page URL and Breadcrumb are displayed for 'Account Logout' page</t>
+  </si>
+  <si>
+    <t>TC_LG_010</t>
+  </si>
+  <si>
+    <t>Validate the UI of the Logout option and the 'Account Logout' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Account' Dropmenu 
+2. Select 'Logout' option (Verify ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for Logout option (My Account DropMenu and Right Column) and 'Account Logout' page</t>
+  </si>
+  <si>
+    <t>TC_LG_011</t>
+  </si>
+  <si>
+    <t>Validate the Logout functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. Logout functionality should work correctly in all the supported environments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,8 +1350,27 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1234,6 +1434,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1412,7 +1624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1488,6 +1700,31 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1508,31 +1745,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1953,7 +2182,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1963,7 +2192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1981,10 +2210,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
@@ -1998,16 +2227,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="34"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="21" t="s">
         <v>30</v>
       </c>
@@ -2025,8 +2254,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -2046,10 +2275,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2071,17 +2300,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
@@ -2116,514 +2345,514 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="33" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:9" s="42" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="28" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="40" t="s">
+      <c r="D8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="27" customFormat="1" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="40" t="s">
+      <c r="D9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="28" customFormat="1" ht="158" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="40" t="s">
+      <c r="D10" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="28" customFormat="1" ht="150.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="40" t="s">
+      <c r="D11" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="28" customFormat="1" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="40" t="s">
+      <c r="D12" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="28" customFormat="1" ht="206" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="40" t="s">
+      <c r="D13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="28" customFormat="1" ht="211.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="44" t="s">
+      <c r="D14" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="28" customFormat="1" ht="218.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="28" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="28" customFormat="1" ht="139" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="28" customFormat="1" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="28" customFormat="1" ht="183" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="D19" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="28" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="40" t="s">
+      <c r="D20" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="28" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="40" t="s">
+      <c r="D21" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="28" customFormat="1" ht="125.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="40" t="s">
+      <c r="D22" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="28" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="40" t="s">
+      <c r="D23" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="28" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="31">
         <v>12345</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="28" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="D25" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="40" t="s">
+      <c r="D25" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="28" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D26" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="40" t="s">
+      <c r="D26" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="G26" s="41" t="s">
+      <c r="G26" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="28" customFormat="1" ht="127" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="D27" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="40" t="s">
+      <c r="D27" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="F27" s="45" t="s">
+      <c r="F27" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="G27" s="41" t="s">
+      <c r="G27" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="28" customFormat="1" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="D28" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="40" t="s">
+      <c r="D28" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="G28" s="41" t="s">
+      <c r="G28" s="33" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="28" customFormat="1" ht="120.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="40" t="s">
+      <c r="D29" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2639,16 +2868,16 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G29">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2669,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2686,603 +2915,603 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="29" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="181" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="42"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="190.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="42"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" ht="195.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="42"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="203" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="42"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="157.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="140" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="40" t="s">
+      <c r="D7" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="42"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="162.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="40" t="s">
+      <c r="D8" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="42"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" ht="171.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="40" t="s">
+      <c r="D9" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="42"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="181" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="G10" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="32" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="32" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="213.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="41" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="32" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="227.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="42"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" ht="140" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="40" t="s">
+      <c r="D14" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="42"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" ht="210" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="42"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" ht="175" x14ac:dyDescent="0.35">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="40" t="s">
+      <c r="D16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="32" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="351" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="42"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" ht="262.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="42"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" ht="213.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="32" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="40" t="s">
+      <c r="D20" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="42"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="D21" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="40" t="s">
+      <c r="D21" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="42"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="40" t="s">
+      <c r="D22" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="42"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" ht="127.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="40" t="s">
+      <c r="D23" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="42"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="172.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="40" t="s">
+      <c r="D24" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="G24" s="41" t="s">
+      <c r="G24" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="42"/>
+      <c r="H24" s="34"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G24">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3293,4 +3522,380 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" width="35.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" customWidth="1"/>
+    <col min="7" max="7" width="34.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="160.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+    </row>
+    <row r="3" spans="1:11" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="4" spans="1:11" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" ht="182.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:11" ht="140" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="1:11" ht="183" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>294</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="49"/>
+    </row>
+    <row r="8" spans="1:11" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="49"/>
+    </row>
+    <row r="9" spans="1:11" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>302</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>303</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="1:11" ht="178" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="1:11" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="F11" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>313</v>
+      </c>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="49"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J12">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+      <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases for forgot password functionality
</commit_message>
<xml_diff>
--- a/OpenCart_TestCases.xlsx
+++ b/OpenCart_TestCases.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Registration_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Login_Page" sheetId="2" r:id="rId2"/>
     <sheet name="Logout_Page" sheetId="3" r:id="rId3"/>
+    <sheet name="ForgotPassword" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="425">
   <si>
     <t>Product Name</t>
   </si>
@@ -1235,12 +1236,407 @@
   <si>
     <t>1. Logout functionality should work correctly in all the supported environments</t>
   </si>
+  <si>
+    <t>TC_FP_001</t>
+  </si>
+  <si>
+    <t>(TS_004)
+Forgot Passsword</t>
+  </si>
+  <si>
+    <t>Validate User is able to reset the password</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and navigate to Login Page
+2. An existing Account is required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Forgotten Password' link from Login page (Validate ER-1)
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button (Validate ER-2)
+4. Check the registered email address for which the password got reset (Validate ER-3)
+5. Click on the link for resseting the password from the received email body (Validate ER-4)
+6. Enter new password into the 'Password' and 'Confirm' fields
+7. Click on 'Continue' button (Validate ER-5)
+8. Enter the email address into the E-Mail address field and the new resetted password into the 'Password' field 
+9. Click on 'Login' button (Validate ER-6)
+</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page
+2. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color
+3. Validate that an email is received regarding resseting of the password to the registered email address 
+4. User should be taken 'Reset your Password' page
+5. Success message with text - 'Success: Your password has been successfully updated.' should be displayed in green color and User should be navigated to 'Login' page
+6. User should be able to login with the new password</t>
+  </si>
+  <si>
+    <t>TC_FP_002</t>
+  </si>
+  <si>
+    <t>Validate an email is sent with the proper details on resetting the password</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page 
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset (Validate ER-1 and ER-2)</t>
+  </si>
+  <si>
+    <t>1. An email should be recevied by the registered email address with the details of resetting the password.
+2. Email should contain proper Subject, Body, from address and the link for resetting the password</t>
+  </si>
+  <si>
+    <t>TC_FP_003</t>
+  </si>
+  <si>
+    <t>Validate logging into the Application with the old password after resetting it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. An existing Account is required and we have reset the password
+2. Open the Application URL and navigate to Login Page
+</t>
+  </si>
+  <si>
+    <t>1. Enter registered email address into the 'E-Mail address' field
+2. Enter new password into the 'Password' field
+3. Click on 'Login' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should not be able to login with old password </t>
+  </si>
+  <si>
+    <t>TC_FP_004</t>
+  </si>
+  <si>
+    <t>Validate logging into the Application with the old password when you have initiated the resetting password process and have not reset the password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL and navigate to Login Page
+1. An existing Account is required 
+</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Enter registered email address into the 'E-mail Address' field
+5. Enter old password into the 'Password' field
+6. Click on 'Login' button</t>
+  </si>
+  <si>
+    <t>1. User should be able to login</t>
+  </si>
+  <si>
+    <t>TC_FP_005</t>
+  </si>
+  <si>
+    <t>Validate resetting the password for a non-registered account</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and navigate to Login Page</t>
+  </si>
+  <si>
+    <t>1.Click on 'Forgotten Password' link from Login page
+2. Enter an email address for which the Account doesn't exist in the application
+3. Click on 'Continue' button</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color</t>
+  </si>
+  <si>
+    <t>TC_FP_006</t>
+  </si>
+  <si>
+    <t>Validate how many times the User is able to reset the password using the reset link sent over email</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset 
+5. Click on the link for resseting the password from the received email body
+6. Enter new password into the 'Password' and 'Confirm' fields
+7. Click on 'Continue' button 
+8. Repeat steps 5 to 7  for 2 to 3 times (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be allowed to use the link sent in the email for resetting the password only once</t>
+  </si>
+  <si>
+    <t>TC_FP_007</t>
+  </si>
+  <si>
+    <t>Validate the User has given the same password into the 'Password' and 'Confirm' fields of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter the email address of an existing account for which you have forgot the password 
+3. Click on 'Continue' button
+4. Check the registered email address for which the password got reset 
+5. Click on the link for resseting the password from the received email body
+6. Enter a password into the 'Password' field 
+7. Enter a different password into the 'Confirm' fields
+8. Click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. A field level warning message with text - 'Password and password confirmation do not match!' should be displayed under 'confirm' field</t>
+  </si>
+  <si>
+    <t>TC_FP_008</t>
+  </si>
+  <si>
+    <t>Validate the placeholders are displayed in the 'Password' and 'Confirm' fields of 'Reset your password' page</t>
+  </si>
+  <si>
+    <t>1. An existing Account is required, we have reset the password for this account and a reset password email is sent to the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check whether the 'Password' and 'Confirm' fields in the 'Reset your Password' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper placeholder texts are displayed inside the 'Password' and 'Confirm' fields of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_009</t>
+  </si>
+  <si>
+    <t>Validate resetting the password without giving the new password in the 'Password' and 'Confirm' fields of 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Don't enter any password into the 'Password' and 'Confirm' fields of the 'Reset your Password' page
+3. Click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - 'Password must be between 4 and 20 characters!' should be displayed for 'Password' field</t>
+  </si>
+  <si>
+    <t>TC_FP_010</t>
+  </si>
+  <si>
+    <t>Validate clicking  'Back' button on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Click on 'Back' button on the 'Reset your Password' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_FP_011</t>
+  </si>
+  <si>
+    <t>Validate 'Right Column' options are displayed in the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check for 'Right Column' options (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'Right Columns' options should be displayed in the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_012</t>
+  </si>
+  <si>
+    <t>Validate the Breadcrumb of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the Breadcrumb (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_013</t>
+  </si>
+  <si>
+    <t>Validate Page Heading, Page URL and Page Title of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the Page Heading, Page URL and Page Title (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_014</t>
+  </si>
+  <si>
+    <t>Validate the UI of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Check the UI of the Page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_015</t>
+  </si>
+  <si>
+    <t>Validate reseting the Password without providing the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Don't enter anything into the 'E-Mail Address' field
+3. Click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - E-Mail must be between 4 and 20 characters!' should be displayed for 'E-Mail Address' field</t>
+  </si>
+  <si>
+    <t>TC_FP_016</t>
+  </si>
+  <si>
+    <t>Verifty Placehold text is displayed in the 'E-Mail Address' field of 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check  Placeholder text for 'E-Mail' Address field (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper Placeholder text is displayed inside the 'E-Mail Address' fields  of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_017</t>
+  </si>
+  <si>
+    <t>Validate 'E-Mail Address' fied on the 'Forgotten Password' page is marked as mandatory</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check  the 'E-Mail' Address field (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'E-Mail' Address field in the 'Forgotten Password' page should be marked as mandatory</t>
+  </si>
+  <si>
+    <t>TC_FP_018</t>
+  </si>
+  <si>
+    <t>Validate entering invalid format email address into the 'E-Mail Address' field of 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Enter any invalid formatted email address into the 'E-Mail Address' field (Validate ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try all below invalid email address formats:
+1) pavanol
+2) pavanol@
+3) pavanol@gmail
+4) pavanol@gmail.
+</t>
+  </si>
+  <si>
+    <t>1. Field level warning message informing the User to provide a valid formatted email address should be displayed</t>
+  </si>
+  <si>
+    <t>TC_FP_019</t>
+  </si>
+  <si>
+    <t>Validate Back button on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Click on 'Back' button  (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Login' page</t>
+  </si>
+  <si>
+    <t>TC_FP_020</t>
+  </si>
+  <si>
+    <t>Validate navigating to 'Forgotten Password' page from 'Right Column' options</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' option from the 'Right Column'  (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Forgotten Password page</t>
+  </si>
+  <si>
+    <t>TC_FP_021</t>
+  </si>
+  <si>
+    <t>Validate Breadcrumb of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check the working of Breadcrumb (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_022</t>
+  </si>
+  <si>
+    <t>Validate the email address provided in the 'E-Mail Address' field of 'Login' page, need to be carry forwarded to the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Enter email address into the 'E-Mail Address' field of the Login page
+2. Click on 'Forgotten Password' link (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page and email address given in the Login page should be displayed in this page by default [Usability point of view]</t>
+  </si>
+  <si>
+    <t>TC_FP_023</t>
+  </si>
+  <si>
+    <t>Validate the UI of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Forgotten Password' link from Login page
+2. Check the UI of the Page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>TC_FP_024</t>
+  </si>
+  <si>
+    <t>Validate the Password entered into the 'Password' and 'Confirm' fields of 'Reset your Password' page is toggled to hide its visibility</t>
+  </si>
+  <si>
+    <t>1. An existing Account is required, we have reset the D1:D25password for this account and a reset password email is sent to the registered email address</t>
+  </si>
+  <si>
+    <t>1. Click on the reset password link available in the email 
+2. Enter any text into 'Password' and 'Confirm' fields on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Text entered into the 'Password' and 'Confirmed' fields should be toggled to hide its visibility (i.e. * or . Symbols should be displayed)</t>
+  </si>
+  <si>
+    <t>TC_FP_025</t>
+  </si>
+  <si>
+    <t>Validate the Password Reset functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL and navigate to Login Page
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Forgotten Password' link from Login page </t>
+  </si>
+  <si>
+    <t>1. Reset Password functionality should work correctly in all the supported environments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1366,6 +1762,25 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -1624,7 +2039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1725,6 +2140,23 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1745,29 +2177,59 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2182,7 +2644,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2210,10 +2672,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
@@ -2227,16 +2689,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="43"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="21" t="s">
         <v>30</v>
       </c>
@@ -2254,8 +2716,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -2275,10 +2737,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2300,17 +2762,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
@@ -2345,8 +2807,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="42" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:9" s="49" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="48" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2868,16 +3330,16 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G29">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2898,7 +3360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3502,16 +3964,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G24">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3543,340 +4005,1094 @@
     <col min="7" max="7" width="34.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="43" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="43" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="43" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="160.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="38" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="40" t="s">
         <v>270</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="F2" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="48" t="s">
+      <c r="F2" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="49"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:11" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="38" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="40" t="s">
         <v>275</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="40" t="s">
         <v>276</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="48" t="s">
+      <c r="F3" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="49"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="178.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="48" t="s">
+      <c r="F4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="40" t="s">
         <v>281</v>
       </c>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="49"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" ht="182.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="F5" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="48" t="s">
+      <c r="F5" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="49"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="140" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="40" t="s">
         <v>287</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="40" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="48" t="s">
+      <c r="F6" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="40" t="s">
         <v>290</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="49"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="183" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="40" t="s">
         <v>294</v>
       </c>
-      <c r="F7" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="48" t="s">
+      <c r="F7" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="40" t="s">
         <v>295</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="49"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="F8" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="48" t="s">
+      <c r="F8" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="49"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:11" ht="192.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="48" t="s">
+      <c r="F9" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="49"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="41"/>
     </row>
     <row r="10" spans="1:11" ht="178" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="38" t="s">
         <v>305</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="40" t="s">
         <v>306</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="40" t="s">
         <v>308</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="48" t="s">
+      <c r="F10" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="49"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="F11" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="48" t="s">
+      <c r="F11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="49"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="39" t="s">
         <v>269</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="F12" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="48" t="s">
+      <c r="F12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="49"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="41"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J12">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+      <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.6328125" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" customWidth="1"/>
+    <col min="4" max="4" width="43.453125" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="34.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="H2" s="57"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="57"/>
+    </row>
+    <row r="3" spans="1:11" ht="169.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="54" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>326</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="118" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>331</v>
+      </c>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="57"/>
+    </row>
+    <row r="5" spans="1:11" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="54" t="s">
+        <v>332</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>335</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="57"/>
+    </row>
+    <row r="6" spans="1:11" ht="175.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>340</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="57"/>
+    </row>
+    <row r="7" spans="1:11" ht="188.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="54" t="s">
+        <v>342</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>344</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>345</v>
+      </c>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="57"/>
+    </row>
+    <row r="8" spans="1:11" ht="170.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>347</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>348</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>349</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="57"/>
+    </row>
+    <row r="9" spans="1:11" ht="126.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="54" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>351</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="57"/>
+    </row>
+    <row r="10" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="54" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>357</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="57"/>
+    </row>
+    <row r="11" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>361</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="57"/>
+    </row>
+    <row r="12" spans="1:11" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>363</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>364</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>365</v>
+      </c>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="57"/>
+    </row>
+    <row r="13" spans="1:11" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="54" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>368</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>369</v>
+      </c>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="57"/>
+    </row>
+    <row r="14" spans="1:11" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="54" t="s">
+        <v>370</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>372</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>373</v>
+      </c>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="57"/>
+    </row>
+    <row r="15" spans="1:11" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="54" t="s">
+        <v>374</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>375</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>352</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>376</v>
+      </c>
+      <c r="F15" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>377</v>
+      </c>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="57"/>
+    </row>
+    <row r="16" spans="1:11" ht="165" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="54" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>379</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="56" t="s">
+        <v>381</v>
+      </c>
+      <c r="H16" s="57"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="57"/>
+    </row>
+    <row r="17" spans="1:11" ht="146.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>383</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>384</v>
+      </c>
+      <c r="F17" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>385</v>
+      </c>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="57"/>
+    </row>
+    <row r="18" spans="1:11" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="54" t="s">
+        <v>386</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>387</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>388</v>
+      </c>
+      <c r="F18" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="57"/>
+    </row>
+    <row r="19" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="54" t="s">
+        <v>390</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>391</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>392</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>393</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>394</v>
+      </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="57"/>
+    </row>
+    <row r="20" spans="1:11" ht="202.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="54" t="s">
+        <v>395</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>396</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>397</v>
+      </c>
+      <c r="F20" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>398</v>
+      </c>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="57"/>
+    </row>
+    <row r="21" spans="1:11" ht="175.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="54" t="s">
+        <v>399</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>400</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>401</v>
+      </c>
+      <c r="F21" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>402</v>
+      </c>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="57"/>
+    </row>
+    <row r="22" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="54" t="s">
+        <v>403</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" s="56" t="s">
+        <v>405</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>406</v>
+      </c>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="57"/>
+    </row>
+    <row r="23" spans="1:11" ht="175" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="54" t="s">
+        <v>407</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>408</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>409</v>
+      </c>
+      <c r="F23" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>410</v>
+      </c>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="57"/>
+    </row>
+    <row r="24" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="54" t="s">
+        <v>411</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>412</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="F24" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="57"/>
+    </row>
+    <row r="25" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="54" t="s">
+        <v>415</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>417</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>418</v>
+      </c>
+      <c r="F25" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="57"/>
+    </row>
+    <row r="26" spans="1:11" ht="189" x14ac:dyDescent="0.35">
+      <c r="A26" s="54" t="s">
+        <v>420</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>421</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>422</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>423</v>
+      </c>
+      <c r="F26" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>424</v>
+      </c>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="57"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
     </cfRule>
@@ -3891,11 +5107,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J26">
       <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases for search functionality
</commit_message>
<xml_diff>
--- a/OpenCart_TestCases.xlsx
+++ b/OpenCart_TestCases.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="289" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Registration_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Login_Page" sheetId="2" r:id="rId2"/>
     <sheet name="Logout_Page" sheetId="3" r:id="rId3"/>
     <sheet name="ForgotPassword" sheetId="4" r:id="rId4"/>
+    <sheet name="Search" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="517">
   <si>
     <t>Product Name</t>
   </si>
@@ -1630,6 +1631,345 @@
   </si>
   <si>
     <t>1. Reset Password functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_SF_001</t>
+  </si>
+  <si>
+    <t>(TS_005)
+Search Functionality</t>
+  </si>
+  <si>
+    <t>Validate searching with an existing Product Name</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Product Name: iMac</t>
+  </si>
+  <si>
+    <t>1. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>TC_SF_002</t>
+  </si>
+  <si>
+    <t>Validate searching with a non existing Product Name</t>
+  </si>
+  <si>
+    <t>1. Enter non existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Product Name: Fitbit</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>TC_SF_003</t>
+  </si>
+  <si>
+    <t>Validate searching without providing any Product Name</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1.'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>TC_SF_004</t>
+  </si>
+  <si>
+    <t>Validate searching for a product after login to the Application</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser
+2. Login to the Application</t>
+  </si>
+  <si>
+    <t>TC_SF_005</t>
+  </si>
+  <si>
+    <t>Validate searching by providing a search criteria which results in mulitple products</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Product Name: Mac</t>
+  </si>
+  <si>
+    <t>1. More than one products should be displayed in the search results page</t>
+  </si>
+  <si>
+    <t>TC_SF_006</t>
+  </si>
+  <si>
+    <t>Validate all the fields in the Search functionality and Search page have placeholders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proper placeholder text is displayed in the below fields:
+- Search text box field
+- Search Criteria text box field
+</t>
+  </si>
+  <si>
+    <t>TC_SF_007</t>
+  </si>
+  <si>
+    <t>Validate searching using 'Search Criteria' field</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any existing product name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Click on 'Search' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_SF_008</t>
+  </si>
+  <si>
+    <t>Validate Search using the text from the product description</t>
+  </si>
+  <si>
+    <t>1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any text from the Product Description into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select 'Search in product descriptions' checkbox option
+5. Click on 'Search' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>Text in Production description of iMac Product:  iLife</t>
+  </si>
+  <si>
+    <t>1. Product having the given text in its description should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>TC_SF_009</t>
+  </si>
+  <si>
+    <t>Validate Search by selecting the category of product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any Product Name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select the correct category of the given Product Name into 'Category' dropdown field - &lt;Refer Test Data&gt;
+5. Click on 'Search' button (Validate ER-1)
+6. Select a wrong category in tthe 'Category' dropdown field - - &lt;Refer Test Data&gt;
+7. Click on 'Search' button (Validate ER-2)
+</t>
+  </si>
+  <si>
+    <t>Product Name: iMac
+Correct Category Name: Mac
+Wrong Category Name: PC</t>
+  </si>
+  <si>
+    <t>1. Product should be successfully displayed in the search results.
+2. 'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>TC_SF_010</t>
+  </si>
+  <si>
+    <t>Validate Search by selecting  to search in subcategories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Don't enter anything into the 'Search' text box field 
+2. Click on the button having search icon 
+3. Enter any Product Name into the 'Search Criteria' text box field - &lt;Refer Test Data&gt;
+4. Select the Parent category of the given Product Name into 'Category' dropdown field - &lt;Refer Test Data&gt;
+5. Click on 'Search' button (Validate ER-1)
+6. Select 'Search in subcategories' checkbox field
+7. Click on 'Search' button (Validate ER-2)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name: iMac
+Parent Category Name: Desktops
+</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page
+2. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>TC_SF_011</t>
+  </si>
+  <si>
+    <t>Validate List and Grid views when only one Product is displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Select 'List' option  (Validate ER-1)
+4. Click on the Image of the Product and name of the product (Validate ER-2)
+5. Repeat Steps 1 to 2 and Select 'Grid' option (Validate ER-3)
+6. Click on the Image of the Product and name of the product (Validate ER-4)</t>
+  </si>
+  <si>
+    <t>1. Single product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+2. User should be navigated to the Product Display Page of the product
+3. Single product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+4. User should be navigated to the Product Display Page of the product</t>
+  </si>
+  <si>
+    <t>TC_SF_012</t>
+  </si>
+  <si>
+    <t>Validate List and Grid views when  multiple Products are displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select 'List' option  (Validate ER-2)
+4. Select 'Grid' option (Validate ER-3)</t>
+  </si>
+  <si>
+    <t>Search Criteria: Mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. More than one products should be displayed in the search results page
+2. Multiple product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+3. Multiple product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+</t>
+  </si>
+  <si>
+    <t>TC_SF_013</t>
+  </si>
+  <si>
+    <t>Validate navigating to Product Compare Page from Search Results page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the 'Product Compare' link (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to the Product Compare Page</t>
+  </si>
+  <si>
+    <t>TC_SF_014</t>
+  </si>
+  <si>
+    <t>Validate User is able to sort the Products displayed in the Search Results</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select serveral options from the 'Sort By' dropdown (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. Products are sorted according to the options selected in the 'Sort By' dropdown field</t>
+  </si>
+  <si>
+    <t>TC_SF_015</t>
+  </si>
+  <si>
+    <t>Validate the User can select how many produts can be displayed in the Search Results</t>
+  </si>
+  <si>
+    <t>1. Enter the search criteria in the 'Search' text box field which can result in mutliple products - &lt;Refer Test Data&gt;
+2. Click on the button having search icon (Validate ER-1)
+3. Select the number of Products to be displayed from the 'Show' dropdown (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. The selected number of products should be displayed in the current search page</t>
+  </si>
+  <si>
+    <t>TC_SF_016</t>
+  </si>
+  <si>
+    <t>Validate 'Search' textbox field and the button having search icon are displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>1. Navigate to all the pages of the Application (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Search box field and the button with 'Search' icon should be displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>TC_SF_017</t>
+  </si>
+  <si>
+    <t>Validate navigating to Search page from the Site Map page</t>
+  </si>
+  <si>
+    <t>1. Click on 'Site Map' link in the footer options
+2. Click on the 'Search' link from the 'Site Map' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Search' page</t>
+  </si>
+  <si>
+    <t>TC_SF_018</t>
+  </si>
+  <si>
+    <t>Validate Breadcrumb of the 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Check whether the Breadcrumb option</t>
+  </si>
+  <si>
+    <t>1. Breakcrumb option should be working correctly</t>
+  </si>
+  <si>
+    <t>TC_SF_019</t>
+  </si>
+  <si>
+    <t>Validate we can use all the options of Search functionality using the Keybaord keys</t>
+  </si>
+  <si>
+    <t>1. Press Tab and Enter keys to perform Search operation and select several options in the Search page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be able to perform Search operation and select several options in the Search page using the Keyboard keys Tab and Enter</t>
+  </si>
+  <si>
+    <t>TC_SF_020</t>
+  </si>
+  <si>
+    <t>Validate Page Heading, Page URL and Page Title of the 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing product name into the 'Search' text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon 
+3. Check the Page Heading, Page URL and Page Title of the 'Search' page</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Search' page</t>
+  </si>
+  <si>
+    <t>TC_SF_021</t>
+  </si>
+  <si>
+    <t>Validate the UI of Search functionality and Search page options</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the complete Search functionality</t>
+  </si>
+  <si>
+    <t>TC_SF_022</t>
+  </si>
+  <si>
+    <t>Validate the Search functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. Search functionality should work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -2157,6 +2497,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2177,31 +2536,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2644,7 +3012,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2672,10 +3040,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
@@ -2689,16 +3057,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="50"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="21" t="s">
         <v>30</v>
       </c>
@@ -2716,8 +3084,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
-      <c r="B3" s="46"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -2737,10 +3105,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2762,17 +3130,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
@@ -2807,8 +3175,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="49" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="48" t="s">
+    <row r="7" spans="1:9" s="56" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="55" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3330,16 +3698,16 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G29">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3964,16 +4332,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G24">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4339,16 +4707,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J12">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="BLOCKED">
       <formula>NOT(ISERROR(SEARCH("BLOCKED",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4366,7 +4734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -4382,717 +4750,1389 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="45" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="45" t="s">
         <v>267</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="45" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="140.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="46" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="48" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="56" t="s">
+      <c r="F2" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="57"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
     </row>
     <row r="3" spans="1:11" ht="169.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="48" t="s">
         <v>324</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="48" t="s">
         <v>325</v>
       </c>
-      <c r="F3" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="56" t="s">
+      <c r="F3" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="48" t="s">
         <v>326</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="57"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="1:11" ht="118" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="46" t="s">
         <v>327</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="48" t="s">
         <v>328</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="48" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="48" t="s">
         <v>330</v>
       </c>
-      <c r="F4" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="56" t="s">
+      <c r="F4" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="48" t="s">
         <v>331</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="57"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="1:11" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="48" t="s">
         <v>333</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="48" t="s">
         <v>335</v>
       </c>
-      <c r="F5" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="56" t="s">
+      <c r="F5" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="57"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="1:11" ht="175.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="48" t="s">
         <v>340</v>
       </c>
-      <c r="F6" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="56" t="s">
+      <c r="F6" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="48" t="s">
         <v>341</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="57"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" spans="1:11" ht="188.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="F7" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="56" t="s">
+      <c r="F7" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="48" t="s">
         <v>345</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="57"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="49"/>
     </row>
     <row r="8" spans="1:11" ht="170.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="48" t="s">
         <v>347</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="48" t="s">
         <v>320</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="48" t="s">
         <v>348</v>
       </c>
-      <c r="F8" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="56" t="s">
+      <c r="F8" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="48" t="s">
         <v>349</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="57"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="49"/>
     </row>
     <row r="9" spans="1:11" ht="126.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="F9" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="56" t="s">
+      <c r="F9" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="57"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="49"/>
     </row>
     <row r="10" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="48" t="s">
         <v>356</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="48" t="s">
         <v>357</v>
       </c>
-      <c r="F10" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="56" t="s">
+      <c r="F10" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="48" t="s">
         <v>358</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="57"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="49"/>
     </row>
     <row r="11" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="48" t="s">
         <v>360</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="48" t="s">
         <v>361</v>
       </c>
-      <c r="F11" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="56" t="s">
+      <c r="F11" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="48" t="s">
         <v>192</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="57"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="49"/>
     </row>
     <row r="12" spans="1:11" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="F12" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="56" t="s">
+      <c r="F12" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="48" t="s">
         <v>365</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="57"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="49"/>
     </row>
     <row r="13" spans="1:11" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="46" t="s">
         <v>366</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="48" t="s">
         <v>367</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="48" t="s">
         <v>368</v>
       </c>
-      <c r="F13" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="56" t="s">
+      <c r="F13" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="48" t="s">
         <v>369</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="57"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="49"/>
     </row>
     <row r="14" spans="1:11" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="48" t="s">
         <v>372</v>
       </c>
-      <c r="F14" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="56" t="s">
+      <c r="F14" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="57"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="49"/>
     </row>
     <row r="15" spans="1:11" ht="137.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="46" t="s">
         <v>374</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="48" t="s">
         <v>375</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="48" t="s">
         <v>376</v>
       </c>
-      <c r="F15" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="56" t="s">
+      <c r="F15" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="48" t="s">
         <v>377</v>
       </c>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="57"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="49"/>
     </row>
     <row r="16" spans="1:11" ht="165" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="48" t="s">
         <v>379</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="48" t="s">
         <v>380</v>
       </c>
-      <c r="F16" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="56" t="s">
+      <c r="F16" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="48" t="s">
         <v>381</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="57"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="49"/>
     </row>
     <row r="17" spans="1:11" ht="146.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="48" t="s">
         <v>383</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="48" t="s">
         <v>384</v>
       </c>
-      <c r="F17" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="56" t="s">
+      <c r="F17" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="48" t="s">
         <v>385</v>
       </c>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="57"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="49"/>
     </row>
     <row r="18" spans="1:11" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="46" t="s">
         <v>386</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="48" t="s">
         <v>387</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="48" t="s">
         <v>388</v>
       </c>
-      <c r="F18" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="56" t="s">
+      <c r="F18" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="48" t="s">
         <v>389</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="57"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="49"/>
     </row>
     <row r="19" spans="1:11" ht="160" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="46" t="s">
         <v>390</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="48" t="s">
         <v>391</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="48" t="s">
         <v>392</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="51" t="s">
         <v>393</v>
       </c>
-      <c r="G19" s="56" t="s">
+      <c r="G19" s="48" t="s">
         <v>394</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="57"/>
-    </row>
-    <row r="20" spans="1:11" ht="202.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="54" t="s">
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="49"/>
+    </row>
+    <row r="20" spans="1:11" ht="54" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
         <v>395</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="48" t="s">
         <v>396</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="F20" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="56" t="s">
+      <c r="F20" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="48" t="s">
         <v>398</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="57"/>
-    </row>
-    <row r="21" spans="1:11" ht="175.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="54" t="s">
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="49"/>
+    </row>
+    <row r="21" spans="1:11" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="48" t="s">
         <v>400</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="48" t="s">
         <v>401</v>
       </c>
-      <c r="F21" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="56" t="s">
+      <c r="F21" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="48" t="s">
         <v>402</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="57"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="49"/>
     </row>
     <row r="22" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="48" t="s">
         <v>404</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="48" t="s">
         <v>405</v>
       </c>
-      <c r="F22" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" s="56" t="s">
+      <c r="F22" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="57"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="49"/>
     </row>
     <row r="23" spans="1:11" ht="175" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="46" t="s">
         <v>407</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="48" t="s">
         <v>409</v>
       </c>
-      <c r="F23" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="56" t="s">
+      <c r="F23" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="48" t="s">
         <v>410</v>
       </c>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="57"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="49"/>
     </row>
     <row r="24" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="46" t="s">
         <v>411</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="48" t="s">
         <v>412</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="48" t="s">
         <v>413</v>
       </c>
-      <c r="F24" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="56" t="s">
+      <c r="F24" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="48" t="s">
         <v>414</v>
       </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="57"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="49"/>
     </row>
     <row r="25" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="46" t="s">
         <v>415</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="48" t="s">
         <v>416</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="D25" s="48" t="s">
         <v>417</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="48" t="s">
         <v>418</v>
       </c>
-      <c r="F25" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="56" t="s">
+      <c r="F25" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="48" t="s">
         <v>419</v>
       </c>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="57"/>
-    </row>
-    <row r="26" spans="1:11" ht="189" x14ac:dyDescent="0.35">
-      <c r="A26" s="54" t="s">
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="49"/>
+    </row>
+    <row r="26" spans="1:11" ht="54" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
         <v>420</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="47" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="48" t="s">
         <v>421</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="48" t="s">
         <v>422</v>
       </c>
-      <c r="E26" s="56" t="s">
+      <c r="E26" s="48" t="s">
         <v>423</v>
       </c>
-      <c r="F26" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="56" t="s">
+      <c r="F26" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="48" t="s">
         <v>424</v>
       </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="57"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="49"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J26">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="NOT TESTED">
+      <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="BLOCKED">
+      <formula>NOT(ISERROR(SEARCH("BLOCKED",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J26">
+      <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.36328125" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" customWidth="1"/>
+    <col min="4" max="4" width="34.36328125" customWidth="1"/>
+    <col min="5" max="5" width="33.453125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" customWidth="1"/>
+    <col min="7" max="7" width="27.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="149" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>427</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="H2" s="49"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="49"/>
+    </row>
+    <row r="3" spans="1:11" ht="144" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="4" spans="1:11" ht="98" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>440</v>
+      </c>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="49"/>
+    </row>
+    <row r="5" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="46" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>443</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:11" ht="148.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>445</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>446</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>447</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>448</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="1:11" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>449</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>450</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>439</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>451</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="49"/>
+    </row>
+    <row r="8" spans="1:11" ht="198.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>452</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>453</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>431</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="49"/>
+    </row>
+    <row r="9" spans="1:11" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>458</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>459</v>
+      </c>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="1:11" ht="176.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="46" t="s">
+        <v>460</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>461</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>463</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>464</v>
+      </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>466</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>467</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>468</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>469</v>
+      </c>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:11" ht="158.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="46" t="s">
+        <v>470</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11" ht="153.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="46" t="s">
+        <v>474</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>476</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>477</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="49"/>
+    </row>
+    <row r="14" spans="1:11" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>479</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>481</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>482</v>
+      </c>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="15" spans="1:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
+        <v>483</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>484</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>447</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="49"/>
+    </row>
+    <row r="16" spans="1:11" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="46" t="s">
+        <v>487</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>488</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>489</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>447</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>490</v>
+      </c>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="49"/>
+    </row>
+    <row r="17" spans="1:11" ht="115" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="46" t="s">
+        <v>491</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>492</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>493</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>494</v>
+      </c>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="49"/>
+    </row>
+    <row r="18" spans="1:11" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="46" t="s">
+        <v>495</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>496</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="49"/>
+    </row>
+    <row r="19" spans="1:11" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="46" t="s">
+        <v>499</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>501</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>502</v>
+      </c>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="49"/>
+    </row>
+    <row r="20" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>504</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>505</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>506</v>
+      </c>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="49"/>
+    </row>
+    <row r="21" spans="1:11" ht="169" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="46" t="s">
+        <v>507</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>508</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>509</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>510</v>
+      </c>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="49"/>
+    </row>
+    <row r="22" spans="1:11" ht="148" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="46" t="s">
+        <v>511</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>512</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E22" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>513</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="49"/>
+    </row>
+    <row r="23" spans="1:11" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="46" t="s">
+        <v>514</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>515</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>429</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>516</v>
+      </c>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="49"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT TESTED">
       <formula>NOT(ISERROR(SEARCH("NOT TESTED",J2)))</formula>
     </cfRule>
@@ -5107,7 +6147,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J23">
       <formula1>"PASS, FAIL, Blocked, Not Tested"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>